<commit_message>
GDB break inside function condition
</commit_message>
<xml_diff>
--- a/Index.xlsx
+++ b/Index.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="27795" windowHeight="12975" activeTab="3"/>
+    <workbookView windowWidth="27795" windowHeight="12975" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="C++" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="26">
   <si>
     <t>Id</t>
   </si>
@@ -53,6 +53,18 @@
   </si>
   <si>
     <t>awk '/from/{flag=1} flag'</t>
+  </si>
+  <si>
+    <t>Breakpoint inside certain stack GDB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Set breakpoint which will break program only when function is being called from specified function along the stack. 'Solution' depicts case where i want to break inside some destructor only when it was called from calc_prices_at_trade function </t>
+  </si>
+  <si>
+    <t>br simex::price_vol_t::~price_vol_t if $_caller_is("simex::THashMapPriceTimePriority::calc_prices_at_trade")</t>
+  </si>
+  <si>
+    <t>https://stackoverflow.com/questions/55356858/can-gdb-set-a-breakpoint-on-a-sequence-of-function-calls</t>
   </si>
   <si>
     <t>Setup SSH server on Windows</t>
@@ -90,10 +102,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -120,39 +132,31 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -166,8 +170,68 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -181,53 +245,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -235,14 +254,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -257,25 +269,175 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -287,157 +449,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -456,6 +468,30 @@
       <top/>
       <bottom style="medium">
         <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -485,6 +521,21 @@
     </border>
     <border>
       <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
       <right style="thin">
@@ -499,36 +550,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top style="thin">
@@ -539,156 +560,147 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="12" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="9" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="12" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1108,23 +1120,25 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.8" defaultRowHeight="15" outlineLevelRow="2" outlineLevelCol="6"/>
+  <sheetFormatPr defaultColWidth="8.8" defaultRowHeight="15" outlineLevelRow="3" outlineLevelCol="6"/>
   <cols>
-    <col min="2" max="2" width="32.2" customWidth="1"/>
-    <col min="3" max="3" width="40.9" customWidth="1"/>
-    <col min="4" max="4" width="41.9" customWidth="1"/>
-    <col min="5" max="5" width="18.7" customWidth="1"/>
-    <col min="6" max="6" width="14.8" customWidth="1"/>
-    <col min="7" max="7" width="24.5" customWidth="1"/>
+    <col min="1" max="1" width="8.8" style="1"/>
+    <col min="2" max="2" width="32.2" style="1" customWidth="1"/>
+    <col min="3" max="3" width="40.9" style="1" customWidth="1"/>
+    <col min="4" max="4" width="41.9" style="1" customWidth="1"/>
+    <col min="5" max="5" width="18.7" style="1" customWidth="1"/>
+    <col min="6" max="6" width="14.8" style="1" customWidth="1"/>
+    <col min="7" max="7" width="24.5" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="8.8" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="1" ht="30" spans="1:7">
+    <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1148,31 +1162,48 @@
       </c>
     </row>
     <row r="2" spans="1:4">
-      <c r="A2">
+      <c r="A2" s="1">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="1" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:4">
-      <c r="A3">
+      <c r="A3" s="1">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="1" t="s">
         <v>11</v>
+      </c>
+    </row>
+    <row r="4" ht="86" customHeight="1" spans="1:6">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -1186,7 +1217,7 @@
   <sheetPr/>
   <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
@@ -1230,22 +1261,22 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" ht="45" spans="1:5">
@@ -1253,16 +1284,16 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Perf tools for Ubuntu
</commit_message>
<xml_diff>
--- a/Index.xlsx
+++ b/Index.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="33">
   <si>
     <t>Id</t>
   </si>
@@ -82,6 +82,15 @@
   </si>
   <si>
     <t>https://stackoverflow.com/questions/375913/how-do-i-profile-c-code-running-on-linux</t>
+  </si>
+  <si>
+    <t>Install perf tools on ubuntu</t>
+  </si>
+  <si>
+    <t>Self explainatory</t>
+  </si>
+  <si>
+    <t>sudo apt-get install linux-tools-common linux-tools-generic linux-tools-`uname -r`</t>
   </si>
   <si>
     <t>Setup SSH server on Windows</t>
@@ -120,9 +129,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -136,6 +145,52 @@
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -165,7 +220,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -174,52 +229,6 @@
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -234,7 +243,37 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -242,36 +281,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -286,85 +295,163 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -376,12 +463,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -394,79 +475,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -477,21 +486,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -519,15 +513,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
@@ -539,6 +524,45 @@
       </top>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -557,23 +581,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -582,142 +591,142 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="28" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="28" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="22" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1137,13 +1146,13 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.8" defaultRowHeight="15" outlineLevelRow="4" outlineLevelCol="6"/>
+  <sheetFormatPr defaultColWidth="8.8" defaultRowHeight="15" outlineLevelRow="5" outlineLevelCol="6"/>
   <cols>
     <col min="1" max="1" width="8.8" style="1"/>
     <col min="2" max="2" width="32.2" style="1" customWidth="1"/>
@@ -1238,6 +1247,20 @@
       </c>
       <c r="F5" s="3" t="s">
         <v>19</v>
+      </c>
+    </row>
+    <row r="6" ht="30" spans="1:4">
+      <c r="A6" s="1">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -1298,22 +1321,22 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" ht="45" spans="1:5">
@@ -1321,16 +1344,16 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>